<commit_message>
[tests] backend tests suite update
</commit_message>
<xml_diff>
--- a/web/fixtures/csv/test_data/carbure_duplicates.xlsx
+++ b/web/fixtures/csv/test_data/carbure_duplicates.xlsx
@@ -36,7 +36,7 @@
     <t xml:space="preserve">production_site_country</t>
   </si>
   <si>
-    <t xml:space="preserve">production_site_reference</t>
+    <t xml:space="preserve">supplier_certificate</t>
   </si>
   <si>
     <t xml:space="preserve">production_site_commissioning_date</t>
@@ -2965,14 +2965,15 @@
   </sheetPr>
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.57"/>

</xml_diff>

<commit_message>
[tests] fix test suite
</commit_message>
<xml_diff>
--- a/web/fixtures/csv/test_data/carbure_duplicates.xlsx
+++ b/web/fixtures/csv/test_data/carbure_duplicates.xlsx
@@ -147,358 +147,358 @@
     <t xml:space="preserve">GB</t>
   </si>
   <si>
+    <t xml:space="preserve">EMHV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000688201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le Super Trader 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000381380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPERATEUR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEANTVERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCC-FR-100001014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1997-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR_002_2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000478887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXXON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOBOKEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORTUGASOIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCC-PT-100001080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BETTERAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000429828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANCHESTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000475837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000182371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCC-FR-100001013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2005-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000309035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betterave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANNE_A_SUCRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canne à sucre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECHETS_ORGANIQUES_MENAGERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déchets organiques ménagers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUMIER_HUMIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fumier humide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUMIER_SEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fumier sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUILES_OU_GRAISSES_ANIMALES_CAT1_CAT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huiles ou graisses animales  (catégorie I et/ou II )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUILES_OU_GRAISSES_ANIMALES_CAT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huiles ou graisses animales  (catégorie III)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUILE_PALME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huile de palme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUILE_ALIMENTAIRE_USAGEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huile alimentaire usagée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDUS_VINIQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résidus viniques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOURNESOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tournesol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLYCERINE_BRUTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glycérine brute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECHETS_BOIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déchets de bois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECHETS_INDUSTRIELS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déchets industriels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALGUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOUES_EPURATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boues d'épuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFFLUENTS_HUILERIES_PALME_RAFLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effluents d'huileries de palme et rafles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAI_TALLOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brai de tallol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAGASSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BALLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balles (enveloppes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Râpes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECHETS_MUNICIPAUX_MELANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déchets municipaux en mélange (Hors déchets ménagers triés)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT_CELLULOSIQUE_NON_ALIMENTAIRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matières cellulosiques d'origine non alimentaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT_LIGNO_CELLULOSIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matières ligno-cellulosiques (Hors grumes de sciage &amp; de placage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Égouts pauvres de 2ème extraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMIDON_RESIDUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amidon résiduel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEIGLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seigle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRITICALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triticale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDUS_DE_BIERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résidus de bière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TALLOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tallol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biogaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biogazole de synthèse (Hors HVO)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUILES_OU_GRAISSES_ANIMALES_CAT1_CAT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000688201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Super Trader 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">269</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000381380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPERATEUR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEANTVERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIMES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCC-FR-100001014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1997-07-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR_002_2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMHV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000478887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXXON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOBOKEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PORTUGASOIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PORTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCC-PT-100001080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-07-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BETTERAVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000429828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANCHESTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000475837</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000182371</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCC-FR-100001013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2005-04-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000309035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betterave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CANNE_A_SUCRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canne à sucre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DECHETS_ORGANIQUES_MENAGERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déchets organiques ménagers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUMIER_HUMIDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fumier humide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUMIER_SEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fumier sec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huiles ou graisses animales  (catégorie I et/ou II )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUILES_OU_GRAISSES_ANIMALES_CAT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huiles ou graisses animales  (catégorie III)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUILE_PALME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huile de palme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUILE_ALIMENTAIRE_USAGEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huile alimentaire usagée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maïs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESIDUS_VINIQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résidus viniques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOJA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOURNESOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tournesol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLYCERINE_BRUTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycérine brute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DECHETS_BOIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déchets de bois</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DECHETS_INDUSTRIELS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déchets industriels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALGUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOUES_EPURATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boues d'épuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EFFLUENTS_HUILERIES_PALME_RAFLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effluents d'huileries de palme et rafles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRAI_TALLOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brai de tallol.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAGASSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bagasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BALLES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balles (enveloppes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAPES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Râpes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DECHETS_MUNICIPAUX_MELANGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déchets municipaux en mélange (Hors déchets ménagers triés)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAT_CELLULOSIQUE_NON_ALIMENTAIRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matières cellulosiques d'origine non alimentaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAT_LIGNO_CELLULOSIQUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matières ligno-cellulosiques (Hors grumes de sciage &amp; de placage)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Égouts pauvres de 2ème extraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMIDON_RESIDUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amidon résiduel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEIGLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seigle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRITICALE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triticale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESIDUS_DE_BIERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résidus de bière</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TALLOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tallol.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biogaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biogazole de synthèse (Hors HVO)</t>
   </si>
   <si>
     <t xml:space="preserve">EMHU</t>
@@ -2972,7 +2972,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T25" activeCellId="0" sqref="T25"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3160,10 +3160,10 @@
         <v>40</v>
       </c>
       <c r="I3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>9</v>
@@ -3196,19 +3196,19 @@
         <v>33</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V3" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X3" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z3" s="0" t="s">
         <v>29</v>
@@ -3231,13 +3231,13 @@
         <v>35112</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>10</v>
@@ -3270,19 +3270,19 @@
         <v>33</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V4" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X4" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>29</v>
@@ -3293,34 +3293,34 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>34978</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>12</v>
@@ -3353,22 +3353,22 @@
         <v>33</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X5" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA5" s="0" t="n">
         <v>0</v>
@@ -3376,31 +3376,31 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>34908</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>9</v>
@@ -3433,7 +3433,7 @@
         <v>33</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V6" s="0" t="s">
         <v>35</v>
@@ -3445,7 +3445,7 @@
         <v>37</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Z6" s="0" t="s">
         <v>39</v>
@@ -3468,13 +3468,13 @@
         <v>35120</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>12</v>
@@ -3507,7 +3507,7 @@
         <v>33</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="V7" s="0" t="s">
         <v>35</v>
@@ -3542,13 +3542,13 @@
         <v>35310</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>9</v>
@@ -3581,7 +3581,7 @@
         <v>33</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V8" s="0" t="s">
         <v>35</v>
@@ -3590,7 +3590,7 @@
         <v>37</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z8" s="0" t="s">
         <v>29</v>
@@ -3601,22 +3601,22 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>34671</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>10</v>
@@ -3649,19 +3649,19 @@
         <v>33</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="V9" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X9" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z9" s="0" t="s">
         <v>29</v>
@@ -3761,10 +3761,10 @@
         <v>40</v>
       </c>
       <c r="I11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>9</v>
@@ -3797,19 +3797,19 @@
         <v>33</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V11" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X11" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z11" s="0" t="s">
         <v>29</v>
@@ -3832,13 +3832,13 @@
         <v>35112</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="J12" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>10</v>
@@ -3871,19 +3871,19 @@
         <v>33</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V12" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X12" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z12" s="0" t="s">
         <v>29</v>
@@ -3894,34 +3894,34 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>34978</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>12</v>
@@ -3954,22 +3954,22 @@
         <v>33</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V13" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X13" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA13" s="0" t="n">
         <v>0</v>
@@ -3977,31 +3977,31 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>34908</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>9</v>
@@ -4034,7 +4034,7 @@
         <v>33</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V14" s="0" t="s">
         <v>35</v>
@@ -4046,7 +4046,7 @@
         <v>37</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Z14" s="0" t="s">
         <v>39</v>
@@ -4069,13 +4069,13 @@
         <v>35120</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>12</v>
@@ -4108,7 +4108,7 @@
         <v>33</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="V15" s="0" t="s">
         <v>35</v>
@@ -4143,13 +4143,13 @@
         <v>35310</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>9</v>
@@ -4182,7 +4182,7 @@
         <v>33</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V16" s="0" t="s">
         <v>35</v>
@@ -4191,7 +4191,7 @@
         <v>37</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z16" s="0" t="s">
         <v>29</v>
@@ -4202,22 +4202,22 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>34671</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>10</v>
@@ -4250,19 +4250,19 @@
         <v>33</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="V17" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X17" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y17" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z17" s="0" t="s">
         <v>29</v>
@@ -4362,10 +4362,10 @@
         <v>40</v>
       </c>
       <c r="I19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>9</v>
@@ -4398,19 +4398,19 @@
         <v>33</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V19" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W19" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X19" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y19" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z19" s="0" t="s">
         <v>29</v>
@@ -4433,13 +4433,13 @@
         <v>35112</v>
       </c>
       <c r="H20" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="J20" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>10</v>
@@ -4472,19 +4472,19 @@
         <v>33</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V20" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X20" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y20" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z20" s="0" t="s">
         <v>29</v>
@@ -4495,34 +4495,34 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>34978</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>12</v>
@@ -4555,22 +4555,22 @@
         <v>33</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V21" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W21" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X21" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y21" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z21" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA21" s="0" t="n">
         <v>0</v>
@@ -4578,31 +4578,31 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>34908</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>9</v>
@@ -4635,7 +4635,7 @@
         <v>33</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V22" s="0" t="s">
         <v>35</v>
@@ -4647,7 +4647,7 @@
         <v>37</v>
       </c>
       <c r="Y22" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Z22" s="0" t="s">
         <v>39</v>
@@ -4670,13 +4670,13 @@
         <v>35120</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K23" s="0" t="n">
         <v>12</v>
@@ -4709,7 +4709,7 @@
         <v>33</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="V23" s="0" t="s">
         <v>35</v>
@@ -4744,13 +4744,13 @@
         <v>35310</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>9</v>
@@ -4783,7 +4783,7 @@
         <v>33</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V24" s="0" t="s">
         <v>35</v>
@@ -4792,7 +4792,7 @@
         <v>37</v>
       </c>
       <c r="Y24" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z24" s="0" t="s">
         <v>29</v>
@@ -4803,22 +4803,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>34671</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>10</v>
@@ -4851,19 +4851,19 @@
         <v>33</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="V25" s="0" t="s">
         <v>35</v>
       </c>
       <c r="W25" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X25" s="0" t="s">
         <v>37</v>
       </c>
       <c r="Y25" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z25" s="0" t="s">
         <v>29</v>
@@ -4891,41 +4891,41 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H19:I19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4933,271 +4933,271 @@
         <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5219,41 +5219,41 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H19:I19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5266,10 +5266,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5378,7 +5378,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>179</v>
@@ -5403,17 +5403,17 @@
   <dimension ref="A1:B252"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H19:I19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5578,7 +5578,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>218</v>
@@ -5594,7 +5594,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>221</v>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>427</v>
@@ -6610,7 +6610,7 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B151" s="0" t="s">
         <v>470</v>
@@ -6690,7 +6690,7 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B161" s="0" t="s">
         <v>488</v>
@@ -6890,7 +6890,7 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B186" s="0" t="s">
         <v>537</v>
@@ -6946,7 +6946,7 @@
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B193" s="0" t="s">
         <v>550</v>
@@ -6970,7 +6970,7 @@
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B196" s="0" t="s">
         <v>555</v>
@@ -7282,7 +7282,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B235" s="0" t="s">
         <v>632</v>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B238" s="0" t="s">
         <v>637</v>
@@ -7443,14 +7443,14 @@
   <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H19:I19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7737,17 +7737,17 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H19:I19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>719</v>
@@ -7854,7 +7854,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>747</v>
@@ -7997,7 +7997,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>784</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>814</v>
@@ -8140,7 +8140,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>819</v>

</xml_diff>